<commit_message>
task 4: (1) final match TRBC code, (2) NLP model
</commit_message>
<xml_diff>
--- a/data/external/sustainable-taxonomy_mod.xlsx
+++ b/data/external/sustainable-taxonomy_mod.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10085" uniqueCount="1507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10152" uniqueCount="1505">
   <si>
     <t xml:space="preserve">About this file</t>
   </si>
@@ -6810,6 +6810,9 @@
     <t xml:space="preserve">TRBC (6)</t>
   </si>
   <si>
+    <t xml:space="preserve">NACE_Macro-sector</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -6833,16 +6836,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">TRBC 1 (6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRBC 2 (6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRBC 3 (6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRBC 4 (6)</t>
+    <t xml:space="preserve">TRBC_6</t>
   </si>
 </sst>
 </file>
@@ -6855,7 +6849,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7063,20 +7057,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -7373,7 +7353,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="127">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7878,15 +7858,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8049,7 +8021,7 @@
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C47:E75 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8252,7 +8224,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I364" activeCellId="1" sqref="C47:E75 I364"/>
+      <selection pane="bottomLeft" activeCell="I364" activeCellId="0" sqref="I364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23813,15 +23785,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C47" activeCellId="0" sqref="C47:E75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.45"/>
@@ -23829,22 +23801,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="110" t="s">
-        <v>27</v>
+        <v>1502</v>
       </c>
       <c r="B1" s="110" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="C1" s="110" t="s">
-        <v>1503</v>
-      </c>
-      <c r="D1" s="110" t="s">
         <v>1504</v>
-      </c>
-      <c r="E1" s="110" t="s">
-        <v>1505</v>
-      </c>
-      <c r="F1" s="110" t="s">
-        <v>1506</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23854,7 +23817,7 @@
       <c r="B2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="117" t="n">
+      <c r="C2" s="126" t="n">
         <v>513010</v>
       </c>
     </row>
@@ -23865,7 +23828,7 @@
       <c r="B3" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="117" t="n">
+      <c r="C3" s="126" t="n">
         <v>513010</v>
       </c>
     </row>
@@ -23876,7 +23839,7 @@
       <c r="B4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="117" t="n">
+      <c r="C4" s="126" t="n">
         <v>513010</v>
       </c>
     </row>
@@ -23887,11 +23850,8 @@
       <c r="B5" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="117" t="n">
+      <c r="C5" s="126" t="n">
         <v>532020</v>
-      </c>
-      <c r="D5" s="117" t="n">
-        <v>541020</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23899,12 +23859,9 @@
         <v>40</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="117" t="n">
-        <v>531010</v>
-      </c>
-      <c r="D6" s="117" t="n">
+        <v>50</v>
+      </c>
+      <c r="C6" s="126" t="n">
         <v>541020</v>
       </c>
     </row>
@@ -23913,10 +23870,10 @@
         <v>40</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="117" t="n">
-        <v>541020</v>
+        <v>49</v>
+      </c>
+      <c r="C7" s="126" t="n">
+        <v>531010</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23924,10 +23881,10 @@
         <v>40</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="117" t="n">
-        <v>513010</v>
+        <v>49</v>
+      </c>
+      <c r="C8" s="126" t="n">
+        <v>541020</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23935,38 +23892,32 @@
         <v>40</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="117" t="n">
-        <v>513010</v>
+        <v>51</v>
+      </c>
+      <c r="C9" s="126" t="n">
+        <v>541020</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="117" t="n">
-        <v>554020</v>
-      </c>
-      <c r="D10" s="117" t="n">
-        <v>554030</v>
+        <v>46</v>
+      </c>
+      <c r="C10" s="126" t="n">
+        <v>513010</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="117" t="n">
-        <v>522010</v>
-      </c>
-      <c r="D11" s="117" t="n">
-        <v>532030</v>
+        <v>45</v>
+      </c>
+      <c r="C11" s="126" t="n">
+        <v>513010</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23974,13 +23925,10 @@
         <v>114</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="117" t="n">
-        <v>522010</v>
-      </c>
-      <c r="D12" s="117" t="n">
-        <v>532030</v>
+        <v>118</v>
+      </c>
+      <c r="C12" s="126" t="n">
+        <v>554020</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23988,91 +23936,76 @@
         <v>114</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="117" t="n">
-        <v>522010</v>
-      </c>
-      <c r="D13" s="117" t="n">
-        <v>532030</v>
+        <v>118</v>
+      </c>
+      <c r="C13" s="126" t="n">
+        <v>554030</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D14" s="117" t="n">
-        <v>591040</v>
+        <v>116</v>
+      </c>
+      <c r="C14" s="126" t="n">
+        <v>522010</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D15" s="117" t="n">
-        <v>591030</v>
+        <v>116</v>
+      </c>
+      <c r="C15" s="126" t="n">
+        <v>532030</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="117" t="n">
-        <v>502010</v>
+        <v>115</v>
+      </c>
+      <c r="C16" s="126" t="n">
+        <v>522010</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D17" s="117" t="n">
-        <v>591030</v>
+        <v>115</v>
+      </c>
+      <c r="C17" s="126" t="n">
+        <v>532030</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="117" t="n">
-        <v>591030</v>
-      </c>
-      <c r="D18" s="117" t="n">
-        <v>591040</v>
+        <v>117</v>
+      </c>
+      <c r="C18" s="126" t="n">
+        <v>522010</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="117" t="n">
-        <v>522010</v>
+        <v>117</v>
+      </c>
+      <c r="C19" s="126" t="n">
+        <v>532030</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24080,10 +24013,10 @@
         <v>64</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="117" t="n">
-        <v>502010</v>
+        <v>84</v>
+      </c>
+      <c r="C20" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24091,12 +24024,9 @@
         <v>64</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D21" s="117" t="n">
+        <v>84</v>
+      </c>
+      <c r="C21" s="126" t="n">
         <v>591040</v>
       </c>
     </row>
@@ -24105,13 +24035,10 @@
         <v>64</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="117" t="n">
+        <v>81</v>
+      </c>
+      <c r="C22" s="126" t="n">
         <v>591010</v>
-      </c>
-      <c r="D22" s="117" t="n">
-        <v>591030</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24119,10 +24046,10 @@
         <v>64</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="117" t="n">
-        <v>502010</v>
+        <v>81</v>
+      </c>
+      <c r="C23" s="126" t="n">
+        <v>591030</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24130,13 +24057,10 @@
         <v>64</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D24" s="117" t="n">
-        <v>591030</v>
+        <v>83</v>
+      </c>
+      <c r="C24" s="126" t="n">
+        <v>502010</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24144,7 +24068,10 @@
         <v>64</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>69</v>
+        <v>82</v>
+      </c>
+      <c r="C25" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24152,7 +24079,10 @@
         <v>64</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>68</v>
+        <v>82</v>
+      </c>
+      <c r="C26" s="126" t="n">
+        <v>591030</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24160,12 +24090,9 @@
         <v>64</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D27" s="117" t="n">
+        <v>79</v>
+      </c>
+      <c r="C27" s="126" t="n">
         <v>591030</v>
       </c>
     </row>
@@ -24174,7 +24101,10 @@
         <v>64</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+      <c r="C28" s="126" t="n">
+        <v>591040</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24182,13 +24112,10 @@
         <v>64</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D29" s="117" t="n">
-        <v>591040</v>
+        <v>80</v>
+      </c>
+      <c r="C29" s="126" t="n">
+        <v>522010</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24196,13 +24123,10 @@
         <v>64</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D30" s="117" t="n">
-        <v>591030</v>
+        <v>77</v>
+      </c>
+      <c r="C30" s="126" t="n">
+        <v>502010</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24210,10 +24134,10 @@
         <v>64</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="117" t="n">
-        <v>502010</v>
+        <v>72</v>
+      </c>
+      <c r="C31" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24221,24 +24145,21 @@
         <v>64</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D32" s="117" t="n">
-        <v>591030</v>
+        <v>72</v>
+      </c>
+      <c r="C32" s="126" t="n">
+        <v>591040</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="117" t="n">
-        <v>591030</v>
+      <c r="B33" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24246,16 +24167,10 @@
         <v>64</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="117" t="n">
-        <v>501030</v>
-      </c>
-      <c r="D34" s="117" t="n">
-        <v>591020</v>
-      </c>
-      <c r="E34" s="117" t="n">
-        <v>591040</v>
+        <v>66</v>
+      </c>
+      <c r="C34" s="126" t="n">
+        <v>591030</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24263,13 +24178,10 @@
         <v>64</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D35" s="117" t="n">
-        <v>591040</v>
+        <v>71</v>
+      </c>
+      <c r="C35" s="126" t="n">
+        <v>502010</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24277,13 +24189,10 @@
         <v>64</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="117" t="n">
+        <v>70</v>
+      </c>
+      <c r="C36" s="126" t="n">
         <v>591010</v>
-      </c>
-      <c r="D36" s="117" t="n">
-        <v>591040</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24291,13 +24200,10 @@
         <v>64</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D37" s="117" t="n">
-        <v>591040</v>
+        <v>70</v>
+      </c>
+      <c r="C37" s="126" t="n">
+        <v>591030</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24305,452 +24211,793 @@
         <v>64</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="117" t="n">
-        <v>591010</v>
-      </c>
-      <c r="D38" s="117" t="n">
-        <v>591040</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C38" s="126"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="24" t="s">
-        <v>726</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>727</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="126"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="24" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="117" t="n">
-        <v>522030</v>
-      </c>
-      <c r="D40" s="117" t="n">
-        <v>572010</v>
+        <v>65</v>
+      </c>
+      <c r="C40" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="24" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="117" t="n">
-        <v>522030</v>
-      </c>
-      <c r="D41" s="117" t="n">
-        <v>551020</v>
-      </c>
-      <c r="E41" s="117" t="n">
-        <v>572010</v>
-      </c>
-      <c r="F41" s="117" t="n">
-        <v>581010</v>
+        <v>65</v>
+      </c>
+      <c r="C41" s="126" t="n">
+        <v>591030</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="117" t="n">
-        <v>512010</v>
-      </c>
-      <c r="D42" s="117" t="n">
-        <v>513020</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C42" s="126"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="117" t="n">
-        <v>512020</v>
+        <v>88</v>
+      </c>
+      <c r="C43" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="117" t="n">
-        <v>511010</v>
+        <v>88</v>
+      </c>
+      <c r="C44" s="126" t="n">
+        <v>591040</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="117" t="n">
-        <v>511010</v>
+        <v>85</v>
+      </c>
+      <c r="C45" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="117" t="n">
-        <v>512010</v>
-      </c>
-      <c r="D46" s="117" t="n">
-        <v>513020</v>
+        <v>85</v>
+      </c>
+      <c r="C46" s="126" t="n">
+        <v>591030</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="C47" s="126" t="n">
         <v>502010</v>
       </c>
-      <c r="D47" s="127" t="n">
-        <v>521020</v>
-      </c>
-      <c r="E47" s="127" t="n">
-        <v>531010</v>
-      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C48" s="126" t="n">
-        <v>511010</v>
+        <v>591010</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C49" s="126" t="n">
-        <v>511010</v>
+        <v>591030</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="C50" s="126" t="n">
-        <v>511010</v>
+        <v>591030</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C51" s="126" t="n">
-        <v>511010</v>
+        <v>501030</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C52" s="126" t="n">
-        <v>511010</v>
+        <v>591020</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="24" t="s">
-        <v>728</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>729</v>
-      </c>
-      <c r="C53" s="128" t="n">
-        <v>522030</v>
+        <v>64</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="126" t="n">
+        <v>591040</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C54" s="126" t="n">
-        <v>524050</v>
+        <v>591010</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C55" s="126" t="n">
-        <v>524050</v>
+        <v>591040</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" s="27" t="s">
-        <v>107</v>
+        <v>64</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>76</v>
       </c>
       <c r="C56" s="126" t="n">
-        <v>522010</v>
+        <v>591010</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="C57" s="126" t="n">
-        <v>522010</v>
+        <v>591040</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C58" s="126" t="n">
-        <v>524050</v>
+        <v>591010</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C59" s="126" t="n">
-        <v>524060</v>
+        <v>591040</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="128" t="n">
-        <v>524060</v>
+        <v>73</v>
+      </c>
+      <c r="C60" s="126" t="n">
+        <v>591010</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="24" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C61" s="128" t="n">
-        <v>524050</v>
+        <v>73</v>
+      </c>
+      <c r="C61" s="126" t="n">
+        <v>591040</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C62" s="128" t="n">
-        <v>524060</v>
-      </c>
+        <v>726</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>727</v>
+      </c>
+      <c r="C62" s="126"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="24" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="128" t="n">
-        <v>524060</v>
+        <v>120</v>
+      </c>
+      <c r="C63" s="126" t="n">
+        <v>522030</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="24" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="128" t="n">
-        <v>522030</v>
+        <v>120</v>
+      </c>
+      <c r="C64" s="126" t="n">
+        <v>572010</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C65" s="128" t="n">
+        <v>119</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="126" t="n">
         <v>522030</v>
-      </c>
-      <c r="D65" s="128" t="n">
-        <v>591030</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="24" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C66" s="128" t="n">
-        <v>522030</v>
+        <v>121</v>
+      </c>
+      <c r="C66" s="126" t="n">
+        <v>551020</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B67" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C67" s="128" t="n">
-        <v>591030</v>
-      </c>
-      <c r="D67" s="128" t="n">
-        <v>591040</v>
+        <v>119</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" s="126" t="n">
+        <v>572010</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="24" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68" s="128" t="n">
-        <v>522030</v>
+        <v>121</v>
+      </c>
+      <c r="C68" s="126" t="n">
+        <v>581010</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="24" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C69" s="128" t="n">
-        <v>522030</v>
+        <v>55</v>
+      </c>
+      <c r="C69" s="126" t="n">
+        <v>512010</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="24" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70" s="128" t="n">
-        <v>522030</v>
+        <v>55</v>
+      </c>
+      <c r="C70" s="126" t="n">
+        <v>513020</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="24" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" s="128" t="n">
-        <v>522030</v>
+        <v>54</v>
+      </c>
+      <c r="C71" s="126" t="n">
+        <v>512020</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="24" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C72" s="128" t="n">
-        <v>522030</v>
+        <v>62</v>
+      </c>
+      <c r="C72" s="126" t="n">
+        <v>511010</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="24" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="128" t="n">
-        <v>522030</v>
+        <v>57</v>
+      </c>
+      <c r="C73" s="126" t="n">
+        <v>511010</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="24" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="C74" s="128" t="n">
-        <v>522030</v>
-      </c>
-      <c r="D74" s="128" t="n">
-        <v>524050</v>
+        <v>56</v>
+      </c>
+      <c r="C74" s="126" t="n">
+        <v>512010</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" s="126" t="n">
+        <v>513020</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" s="126" t="n">
+        <v>502010</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="126" t="n">
+        <v>521020</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="126" t="n">
+        <v>531010</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" s="126" t="n">
+        <v>511010</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C80" s="126" t="n">
+        <v>511010</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="126" t="n">
+        <v>511010</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="126" t="n">
+        <v>511010</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B83" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" s="126" t="n">
+        <v>511010</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="24" t="s">
+        <v>728</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>729</v>
+      </c>
+      <c r="C84" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C85" s="126" t="n">
+        <v>524050</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" s="126" t="n">
+        <v>524050</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C87" s="126" t="n">
+        <v>522010</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C88" s="126" t="n">
+        <v>522010</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C89" s="126" t="n">
+        <v>524050</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" s="126" t="n">
+        <v>524060</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" s="126" t="n">
+        <v>524060</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" s="126" t="n">
+        <v>524050</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B93" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C93" s="126" t="n">
+        <v>524060</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" s="126" t="n">
+        <v>524060</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="B95" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B96" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C97" s="126" t="n">
+        <v>591030</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" s="126" t="n">
+        <v>591030</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B100" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C100" s="126" t="n">
+        <v>591040</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B101" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C101" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C102" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B103" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C103" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B104" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C104" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B105" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C105" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B106" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C106" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B107" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C107" s="126" t="n">
+        <v>522030</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C108" s="126" t="n">
+        <v>524050</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B109" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C75" s="128" t="n">
+      <c r="C109" s="126" t="n">
         <v>591030</v>
       </c>
-      <c r="D75" s="128" t="n">
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C110" s="126" t="n">
         <v>591040</v>
       </c>
     </row>
@@ -24777,10 +25024,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
-      <selection pane="bottomRight" activeCell="B67" activeCellId="1" sqref="C47:E75 B67"/>
+      <selection pane="bottomRight" activeCell="B67" activeCellId="0" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="52.85"/>
@@ -27048,10 +27295,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F19" activeCellId="1" sqref="C47:E75 F19"/>
+      <selection pane="bottomRight" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="30" width="10.43"/>
@@ -31669,7 +31916,7 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="1" sqref="C47:E75 A72"/>
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33422,7 +33669,7 @@
   <dimension ref="A1:W70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="1" sqref="C47:E75 E25"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37557,7 +37804,7 @@
   <dimension ref="B2:C28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="C47:E75 F8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37770,7 +38017,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="C47:E75 A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38313,7 +38560,7 @@
   <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C47:E75 D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39735,7 +39982,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D135" activeCellId="1" sqref="C47:E75 D135"/>
+      <selection pane="bottomLeft" activeCell="D135" activeCellId="0" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>